<commit_message>
Actualizando monitoreo de riesgos
</commit_message>
<xml_diff>
--- a/Deliverables/2) Planning/Matriz_Riesgos.xlsx
+++ b/Deliverables/2) Planning/Matriz_Riesgos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valdemar\Documents\Diplomado_SWEmbebido\_GIT_PI_DSW_UTEQ_GE\PI_DSW_UTEQ_GE\ProjectManagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valdemar\Documents\Diplomado_SWEmbebido\_GIT_PI_DSW_UTEQ_GE\PI_DSW_UTEQ_GE\Deliverables\2) Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7574BDF1-AC7E-423B-81E4-C5102F3C3AED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E29A92-90E7-4391-9550-B25CC8E95DA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t xml:space="preserve">RIESGO </t>
   </si>
@@ -181,9 +181,6 @@
 [23/Julio] Se encuentra error y se ajusta requisito para hacer lecturas correctas.</t>
   </si>
   <si>
-    <t>[26/Julio] No ha sucedido el riesgo.</t>
-  </si>
-  <si>
     <t>[12/Julio] Cambio en fecha de entrega, nueva definición de documentación y cambios menores en requisitos.
 [19/Julio] Se solicita prórroga para entrega de proyecto.
 [23/Julio] Se acepta prórroga. Se ajusta documento de requisitos y fechas de entrega considerando documentación a entregar.</t>
@@ -196,6 +193,13 @@
   <si>
     <t>[28/Junio] Se hacen pruebas con potenciómetro, motor, Puente-H, Sensor. No hay daño en los componentes.
 [26/Julio] No ha sucedido el riesgo.</t>
+  </si>
+  <si>
+    <t>Se evaluará la posibilidad de utilizar un controlador más simple al PID, como un PI o P.</t>
+  </si>
+  <si>
+    <t>[26/Julio] El controlador de tipo PID no se comporta de la manera esperada.
+[07/Ago] No se ha logrado hacer funcionar el controlador al integrarlo en el sistema. Se decidió buscar una alternativa al PID y completar esta implementación posteriormente.</t>
   </si>
 </sst>
 </file>
@@ -320,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -377,9 +381,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -843,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -976,7 +977,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
@@ -997,10 +998,10 @@
         <v>24</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1027,7 +1028,7 @@
         <v>42</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="87" thickBot="1" x14ac:dyDescent="0.35">
@@ -1054,7 +1055,7 @@
         <v>42</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="87" thickBot="1" x14ac:dyDescent="0.35">
@@ -1081,7 +1082,7 @@
         <v>43</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>